<commit_message>
add 2.4, 2.5 and 2.6
</commit_message>
<xml_diff>
--- a/2.4.xlsx
+++ b/2.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerej\jotu-pro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5599526-F8AE-4594-96E0-F10B0DB5CC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC5B4EA-ACCD-4931-B7A5-FDB6214B48AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DB093377-F6B0-49E6-8107-7181D39AEF5A}"/>
   </bookViews>
@@ -113,9 +113,6 @@
     <t>Haastattelu</t>
   </si>
   <si>
-    <t>Asiakkaat</t>
-  </si>
-  <si>
     <t>Sisällöntuottaja</t>
   </si>
   <si>
@@ -153,13 +150,16 @@
   </si>
   <si>
     <t>Ylläpitävät sovellusta</t>
+  </si>
+  <si>
+    <t>Voiman asiakkaat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,7 +169,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -265,16 +272,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -285,7 +292,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -604,36 +614,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C062DE-959D-467C-B4D1-4AC09E6CC5EA}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="7" width="30.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -642,151 +655,152 @@
       <c r="F2" s="5"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="F5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>35</v>
+      <c r="G7" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="8" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="B8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="E8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="87" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="3"/>
+      <c r="B9" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "add 2.4, 2.5 and 2.6"
This reverts commit d45a3b57618baa10a06c81af82bdcc39fc0e60d1.
</commit_message>
<xml_diff>
--- a/2.4.xlsx
+++ b/2.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerej\jotu-pro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC5B4EA-ACCD-4931-B7A5-FDB6214B48AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5599526-F8AE-4594-96E0-F10B0DB5CC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DB093377-F6B0-49E6-8107-7181D39AEF5A}"/>
   </bookViews>
@@ -113,6 +113,9 @@
     <t>Haastattelu</t>
   </si>
   <si>
+    <t>Asiakkaat</t>
+  </si>
+  <si>
     <t>Sisällöntuottaja</t>
   </si>
   <si>
@@ -150,16 +153,13 @@
   </si>
   <si>
     <t>Ylläpitävät sovellusta</t>
-  </si>
-  <si>
-    <t>Voiman asiakkaat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,14 +169,7 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -272,16 +265,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -292,10 +285,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -614,39 +604,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C062DE-959D-467C-B4D1-4AC09E6CC5EA}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="7" width="30.6328125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -655,152 +642,151 @@
       <c r="F2" s="5"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="C8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="7" t="s">
+      <c r="E8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="1"/>
+      <c r="B9" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>